<commit_message>
some minor modifications and one comment
git-svn-id: file://localhost/tmp/svn2git/svn@3006 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/cloudcom10/performance/startup.xlsx
+++ b/papers/cloudcom10/performance/startup.xlsx
@@ -171,7 +171,17 @@
   <c:style val="1"/>
   <c:chart>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.158003937007874"/>
+          <c:y val="0.0620366724992709"/>
+          <c:w val="0.81144050743657"/>
+          <c:h val="0.670834062408865"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
@@ -205,7 +215,7 @@
                   <c:v>1.744166666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -241,7 +251,7 @@
                   <c:v>1.51045613944562</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -298,7 +308,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.176786526684164"/>
+          <c:y val="0.893915864683581"/>
+          <c:w val="0.651982502187227"/>
+          <c:h val="0.106084135316419"/>
+        </c:manualLayout>
+      </c:layout>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -895,7 +914,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -986,7 +1005,7 @@
         <v>1.7441666666666669</v>
       </c>
       <c r="F9">
-        <v>2.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1004,8 +1023,7 @@
         <v>1.51045613944562</v>
       </c>
       <c r="F10">
-        <f>5-2.8</f>
-        <v>2.2000000000000002</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:7">

</xml_diff>

<commit_message>
refined sub-job startup time graph; minor modifications
git-svn-id: file://localhost/tmp/svn2git/svn@3007 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/cloudcom10/performance/startup.xlsx
+++ b/papers/cloudcom10/performance/startup.xlsx
@@ -20,91 +20,107 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Exp #</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Time</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>QB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Mean</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>stddev</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>std err</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Azure sub-job startup</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Spawn Time</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>avg</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>stddev</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Time-to-start</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Azure</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>grid</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Azure</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Grid</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Grid</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Submit</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Time-to-Start</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>avg</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Azure (without staging)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>std</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="174" formatCode="0.0"/>
-    <numFmt numFmtId="176" formatCode="0.0000000"/>
-    <numFmt numFmtId="177" formatCode="0.00"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -147,14 +163,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -212,7 +231,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1.744166666666667</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.0</c:v>
@@ -227,6 +246,40 @@
           <c:tx>
             <c:v>Time-to-Start</c:v>
           </c:tx>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(Azure!$B$50,Azure!$B$28)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.231983712971547</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(Azure!$B$50,Azure!$B$28)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.231983712971547</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Azure!$E$8:$F$8</c:f>
@@ -248,7 +301,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1.51045613944562</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.5</c:v>
@@ -258,24 +311,24 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="600171128"/>
-        <c:axId val="599948920"/>
+        <c:axId val="703683368"/>
+        <c:axId val="703687400"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="600171128"/>
+        <c:axId val="703683368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="599948920"/>
+        <c:crossAx val="703687400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="599948920"/>
+        <c:axId val="703687400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -301,7 +354,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="600171128"/>
+        <c:crossAx val="703683368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -898,9 +951,9 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -911,10 +964,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -951,7 +1004,7 @@
       </c>
       <c r="F3">
         <f>A27</f>
-        <v>2.8</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -1002,7 +1055,7 @@
         <v>16</v>
       </c>
       <c r="E9">
-        <v>1.7441666666666669</v>
+        <v>0.9</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1019,8 +1072,8 @@
         <v>17</v>
       </c>
       <c r="E10">
-        <f>2.51045613944562-1</f>
-        <v>1.51045613944562</v>
+        <f>1.5-E9</f>
+        <v>0.6</v>
       </c>
       <c r="F10">
         <v>0.5</v>
@@ -1132,26 +1185,173 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>2.8</v>
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>1.5</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28">
-        <v>1.24</v>
+      <c r="B28">
+        <v>0</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="7">
+        <v>0.78</v>
+      </c>
+      <c r="B35" s="7">
+        <v>1.494</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="7">
+        <v>0.78430999999999995</v>
+      </c>
+      <c r="B36" s="7">
+        <v>1.3751</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="7">
+        <v>1.02</v>
+      </c>
+      <c r="B37" s="7">
+        <v>2.17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="7">
+        <v>0.79</v>
+      </c>
+      <c r="B38" s="7">
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="7">
+        <v>0.79788588999999999</v>
+      </c>
+      <c r="B39" s="7">
+        <v>1.389</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="7">
+        <v>0.89</v>
+      </c>
+      <c r="B40" s="7">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="7">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="B41" s="7">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="7">
+        <v>0.78232000000000002</v>
+      </c>
+      <c r="B42">
+        <v>1.36</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="7">
+        <v>0.83899999999999997</v>
+      </c>
+      <c r="B43" s="7">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="7">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="B44" s="7">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="7">
+        <v>0.78</v>
+      </c>
+      <c r="B45" s="7">
+        <v>1.4775</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="7">
+        <v>0.80296000000000001</v>
+      </c>
+      <c r="B46" s="7">
+        <v>1.7481899999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="7">
+        <v>0.84</v>
+      </c>
+      <c r="B47" s="7">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="7">
+        <v>0.79</v>
+      </c>
+      <c r="B48" s="7">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="3" customFormat="1">
+      <c r="A49" s="8">
+        <f>AVERAGE(A35:A48)</f>
+        <v>0.85174827785714291</v>
+      </c>
+      <c r="B49" s="8">
+        <f>AVERAGE(B35:B48)</f>
+        <v>1.5377707142857144</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="9">
+        <f>STDEV(A35:A48)</f>
+        <v>0.10458953098976645</v>
+      </c>
+      <c r="B50" s="9">
+        <f>STDEV(B35:B48)</f>
+        <v>0.23198371297154677</v>
+      </c>
+      <c r="C50" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A26:B26"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
refined submission time analysis
git-svn-id: file://localhost/tmp/svn2git/svn@3021 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/cloudcom10/performance/startup.xlsx
+++ b/papers/cloudcom10/performance/startup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="20740" windowHeight="15400" tabRatio="500"/>
+    <workbookView xWindow="-25860" yWindow="-520" windowWidth="20740" windowHeight="15400" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Grid" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Time to Subjob Start</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -30,10 +30,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>End Time</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>Time-To-Start (in sec)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -135,6 +131,18 @@
   </si>
   <si>
     <t>Abhinav</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>End Time (Running)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>End Time (Submission)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Submission Time (in sec)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -142,10 +150,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.000000000"/>
-    <numFmt numFmtId="173" formatCode="0.00"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -201,7 +207,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -211,10 +217,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -275,7 +282,7 @@
                   <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>0.17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -292,30 +299,24 @@
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>(Azure!$B$50,Azure!$B$28)</c:f>
+                <c:f>Grid!$E$40</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
+                  <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>0.231983712971547</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.616894295144472</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>(Azure!$B$50,Azure!$B$28)</c:f>
+                <c:f>Grid!$E$40</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="2"/>
+                  <c:ptCount val="1"/>
                   <c:pt idx="0">
-                    <c:v>0.231983712971547</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.0</c:v>
+                    <c:v>0.616894295144472</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -339,37 +340,37 @@
             <c:numRef>
               <c:f>Azure!$E$10:$F$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
+                <c:pt idx="0" formatCode="General">
                   <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>1.43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="567686520"/>
-        <c:axId val="567677304"/>
+        <c:axId val="621097928"/>
+        <c:axId val="74198744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="567686520"/>
+        <c:axId val="621097928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="567677304"/>
+        <c:crossAx val="74198744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="567677304"/>
+        <c:axId val="74198744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -395,7 +396,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="567686520"/>
+        <c:crossAx val="621097928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -795,34 +796,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="10" t="s">
-        <v>28</v>
+      <c r="A1" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -857,7 +859,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -892,7 +894,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>2.8</v>
@@ -927,7 +929,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
         <v>1.2489995996796797</v>
@@ -962,7 +964,7 @@
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <f>B8/SQRT(10)</f>
@@ -1010,264 +1012,412 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:5">
+      <c r="A18" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="11">
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="10">
         <v>10.0916628838</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="1">
+        <v>10.284512042999999</v>
+      </c>
+      <c r="C19" s="10">
         <v>10.8655810356</v>
       </c>
-      <c r="C19" s="12">
+      <c r="D19" s="13">
         <f>B19-A19</f>
+        <v>0.19284915919999968</v>
+      </c>
+      <c r="E19" s="11">
+        <f>C19-A19</f>
         <v>0.77391815180000023</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="11">
+    <row r="20" spans="1:5">
+      <c r="A20" s="10">
         <v>10.865599870700001</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
+        <v>11.047404050800001</v>
+      </c>
+      <c r="C20">
         <v>11.6859428883</v>
       </c>
-      <c r="C20" s="12">
-        <f t="shared" ref="C20:C37" si="1">B20-A20</f>
+      <c r="D20" s="13">
+        <f t="shared" ref="D20:D37" si="1">B20-A20</f>
+        <v>0.18180418010000032</v>
+      </c>
+      <c r="E20" s="11">
+        <f>C20-A20</f>
         <v>0.82034301759999906</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>11.6859660149</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
+        <v>11.8699538708</v>
+      </c>
+      <c r="C21">
         <v>12.474107980699999</v>
       </c>
-      <c r="C21" s="12">
+      <c r="D21" s="13">
         <f t="shared" si="1"/>
+        <v>0.18398785589999989</v>
+      </c>
+      <c r="E21" s="11">
+        <f>C21-A21</f>
         <v>0.78814196579999951</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>12.474129915200001</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
+        <v>12.655675888099999</v>
+      </c>
+      <c r="C22">
         <v>13.361081838600001</v>
       </c>
-      <c r="C22" s="12">
+      <c r="D22" s="13">
         <f t="shared" si="1"/>
+        <v>0.18154597289999863</v>
+      </c>
+      <c r="E22" s="11">
+        <f>C22-A22</f>
         <v>0.88695192339999984</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>13.3611018658</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
+        <v>13.547494888299999</v>
+      </c>
+      <c r="C23">
         <v>14.366608858099999</v>
       </c>
-      <c r="C23" s="12">
+      <c r="D23" s="13">
         <f t="shared" si="1"/>
+        <v>0.18639302249999901</v>
+      </c>
+      <c r="E23" s="11">
+        <f>C23-A23</f>
         <v>1.0055069922999991</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>14.3666298389</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
+        <v>14.5316648483</v>
+      </c>
+      <c r="C24">
         <v>15.4869689941</v>
       </c>
-      <c r="C24" s="12">
+      <c r="D24" s="13">
         <f t="shared" si="1"/>
+        <v>0.16503500940000038</v>
+      </c>
+      <c r="E24" s="11">
+        <f>C24-A24</f>
         <v>1.1203391551999999</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>15.486990928599999</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
+        <v>15.6650369167</v>
+      </c>
+      <c r="C25">
         <v>16.733777999899999</v>
       </c>
-      <c r="C25" s="12">
+      <c r="D25" s="13">
         <f t="shared" si="1"/>
+        <v>0.17804598810000094</v>
+      </c>
+      <c r="E25" s="11">
+        <f>C25-A25</f>
         <v>1.2467870713</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>16.733809948000001</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
+        <v>16.9130840302</v>
+      </c>
+      <c r="C26">
         <v>18.090980052900001</v>
       </c>
-      <c r="C26" s="12">
+      <c r="D26" s="13">
         <f t="shared" si="1"/>
+        <v>0.17927408219999919</v>
+      </c>
+      <c r="E26" s="11">
+        <f>C26-A26</f>
         <v>1.3571701048999998</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>18.091001033800001</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
+        <v>18.257091999099998</v>
+      </c>
+      <c r="C27">
         <v>19.556478023499999</v>
       </c>
-      <c r="C27" s="12">
+      <c r="D27" s="13">
         <f t="shared" si="1"/>
+        <v>0.1660909652999969</v>
+      </c>
+      <c r="E27" s="11">
+        <f>C27-A27</f>
         <v>1.4654769896999973</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>19.556499958</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
+        <v>19.739265918699999</v>
+      </c>
+      <c r="C28">
         <v>21.141931057000001</v>
       </c>
-      <c r="C28" s="12">
+      <c r="D28" s="13">
         <f t="shared" si="1"/>
+        <v>0.1827659606999994</v>
+      </c>
+      <c r="E28" s="11">
+        <f>C28-A28</f>
         <v>1.5854310990000009</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>21.141952991499998</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
+        <v>21.3002460003</v>
+      </c>
+      <c r="C29">
         <v>22.832988023799999</v>
       </c>
-      <c r="C29" s="12">
+      <c r="D29" s="13">
         <f t="shared" si="1"/>
+        <v>0.15829300880000119</v>
+      </c>
+      <c r="E29" s="11">
+        <f>C29-A29</f>
         <v>1.6910350323000003</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>22.833010911900001</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
+        <v>23.009665966</v>
+      </c>
+      <c r="C30">
         <v>24.652971983</v>
       </c>
-      <c r="C30" s="12">
+      <c r="D30" s="13">
         <f t="shared" si="1"/>
+        <v>0.17665505409999938</v>
+      </c>
+      <c r="E30" s="11">
+        <f>C30-A30</f>
         <v>1.8199610710999998</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>24.652993917500002</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
+        <v>24.815809011500001</v>
+      </c>
+      <c r="C31">
         <v>26.5726368427</v>
       </c>
-      <c r="C31" s="12">
+      <c r="D31" s="13">
         <f t="shared" si="1"/>
+        <v>0.16281509399999905</v>
+      </c>
+      <c r="E31" s="11">
+        <f>C31-A31</f>
         <v>1.919642925199998</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>26.572658061999999</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
+        <v>26.7473399639</v>
+      </c>
+      <c r="C32">
         <v>28.610350847199999</v>
       </c>
-      <c r="C32" s="12">
+      <c r="D32" s="13">
         <f t="shared" si="1"/>
+        <v>0.17468190190000144</v>
+      </c>
+      <c r="E32" s="11">
+        <f>C32-A32</f>
         <v>2.0376927852000009</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>28.610369920699998</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
+        <v>28.769356012300001</v>
+      </c>
+      <c r="C33">
         <v>30.778532028200001</v>
       </c>
-      <c r="C33" s="12">
+      <c r="D33" s="13">
         <f t="shared" si="1"/>
+        <v>0.15898609160000277</v>
+      </c>
+      <c r="E33" s="11">
+        <f>C33-A33</f>
         <v>2.1681621075000024</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>30.778554916400001</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
+        <v>30.965348959</v>
+      </c>
+      <c r="C34">
         <v>33.042562961599998</v>
       </c>
-      <c r="C34" s="12">
+      <c r="D34" s="13">
         <f t="shared" si="1"/>
+        <v>0.18679404259999899</v>
+      </c>
+      <c r="E34" s="11">
+        <f>C34-A34</f>
         <v>2.2640080451999971</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>33.042587041899999</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
+        <v>33.220833063100002</v>
+      </c>
+      <c r="C35">
         <v>35.419716835000003</v>
       </c>
-      <c r="C35" s="12">
+      <c r="D35" s="13">
         <f t="shared" si="1"/>
+        <v>0.17824602120000321</v>
+      </c>
+      <c r="E35" s="11">
+        <f>C35-A35</f>
         <v>2.3771297931000035</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>35.419739961600001</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
+        <v>35.559836864499999</v>
+      </c>
+      <c r="C36">
         <v>37.9431979656</v>
       </c>
-      <c r="C36" s="12">
+      <c r="D36" s="13">
         <f t="shared" si="1"/>
+        <v>0.1400969028999981</v>
+      </c>
+      <c r="E36" s="11">
+        <f>C36-A36</f>
         <v>2.5234580039999983</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>37.943222045900001</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
+        <v>38.131721973399998</v>
+      </c>
+      <c r="C37">
         <v>40.561116933800001</v>
       </c>
-      <c r="C37" s="12">
+      <c r="D37" s="13">
         <f t="shared" si="1"/>
+        <v>0.188499927499997</v>
+      </c>
+      <c r="E37" s="11">
+        <f>C37-A37</f>
         <v>2.6178948879000004</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="B39" t="s">
+    <row r="39" spans="1:5">
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="11">
+        <f>AVERAGE(D19:D37)</f>
+        <v>0.17488738109999977</v>
+      </c>
+      <c r="E39" s="11">
+        <f>AVERAGE(E19:E37)</f>
+        <v>1.6036342696052628</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="C40" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="12">
-        <f>AVERAGE(C19:C37)</f>
-        <v>1.6036342696052628</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="B40" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40">
-        <f>STDEV(C19:C37)</f>
+      <c r="D40">
+        <f>STDEV(D19:D37)</f>
+        <v>1.3168987181579812E-2</v>
+      </c>
+      <c r="E40">
+        <f>STDEV(E19:E37)</f>
         <v>0.61689429514447258</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="10" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1283,24 +1433,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="9"/>
+      <c r="A2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="12"/>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2">
         <v>1.7441666666666669</v>
@@ -1311,13 +1461,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3">
         <f>A27</f>
@@ -1355,10 +1505,10 @@
         <v>3.4789741039300002</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1369,13 +1519,13 @@
         <v>3.0715618133499998</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9">
         <v>0.9</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1386,14 +1536,15 @@
         <v>2.65</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10">
         <f>1.5-E9</f>
         <v>0.6</v>
       </c>
-      <c r="F10">
-        <v>0.5</v>
+      <c r="F10" s="11">
+        <f>1.6-F9</f>
+        <v>1.4300000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1478,7 +1629,7 @@
         <v>2.5104561394456248</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1491,14 +1642,14 @@
         <v>0.53691397087472403</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="9"/>
+      <c r="A26" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="12"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
@@ -1508,7 +1659,7 @@
         <v>1.5</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -1516,12 +1667,12 @@
         <v>0</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1646,7 +1797,7 @@
         <v>1.5377707142857144</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1659,10 +1810,11 @@
         <v>0.23198371297154677</v>
       </c>
       <c r="C50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A26:B26"/>

</xml_diff>